<commit_message>
chef mapping DB design
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="184">
   <si>
     <t>RoleName</t>
   </si>
@@ -229,18 +229,6 @@
     <t>TaskStatusId</t>
   </si>
   <si>
-    <t>ChefOrder</t>
-  </si>
-  <si>
-    <t>ChefOrderId</t>
-  </si>
-  <si>
-    <t>MapOrderID</t>
-  </si>
-  <si>
-    <t>ChefDeliveredDateTime</t>
-  </si>
-  <si>
     <t>PaymentType</t>
   </si>
   <si>
@@ -265,18 +253,6 @@
     <t>NumberOfMeal</t>
   </si>
   <si>
-    <t>MapOrderToChef</t>
-  </si>
-  <si>
-    <t>AssignedPickUpDate</t>
-  </si>
-  <si>
-    <t>AssignedPickUpTime</t>
-  </si>
-  <si>
-    <t>OrderGivenDatetime</t>
-  </si>
-  <si>
     <t>Ex:Delivery PointSelected,  Meal Selection in progress, Meal Selected, delivery detail in progress, delivery details entered,  Proceed for Payment, Payment option selected, Payment in progress, confirmed, mapping chef, chef mapped, chef rejected, chef remapped,  food proceed, food collected, delivery in progress, delivered, feed back received.</t>
   </si>
   <si>
@@ -572,6 +548,30 @@
   </si>
   <si>
     <t>Ex:Order Initiated, CoDPayment inprogress, sodexo payment inprogress, NEFT payment inprogress, Paid, confirmed,Cancelling in progress,Cancelled, Meal Planner order in progress, delivery in progress, delivered</t>
+  </si>
+  <si>
+    <t>ChefOrderMapping</t>
+  </si>
+  <si>
+    <t>MappingId</t>
+  </si>
+  <si>
+    <t>OrderGivenTime</t>
+  </si>
+  <si>
+    <t>ExpectedPickupTime</t>
+  </si>
+  <si>
+    <t>ActualPickupTime</t>
+  </si>
+  <si>
+    <t>ChefOrderCancelDetail</t>
+  </si>
+  <si>
+    <t>OrderCanceld</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -955,25 +955,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -988,7 +988,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -997,7 +997,7 @@
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1020,12 +1020,12 @@
         <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -1148,81 +1148,81 @@
     </row>
     <row r="12" spans="1:8" ht="15">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="F16" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1257,32 +1257,32 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
@@ -1320,10 +1320,10 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1331,7 +1331,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -1357,7 +1357,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -1435,7 +1435,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="G8" t="s">
         <v>4</v>
@@ -1458,7 +1458,7 @@
         <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G9" t="s">
         <v>33</v>
@@ -1504,23 +1504,23 @@
         <v>33</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="L15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="N15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="L16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="N16" t="s">
         <v>51</v>
@@ -1528,10 +1528,10 @@
     </row>
     <row r="17" spans="1:14">
       <c r="L17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1552,25 +1552,25 @@
     </row>
     <row r="20" spans="1:14" ht="15">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="L20" t="s">
         <v>3</v>
@@ -1581,22 +1581,22 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" t="s">
-        <v>122</v>
-      </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="L21" t="s">
         <v>4</v>
@@ -1607,22 +1607,22 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" t="s">
         <v>115</v>
       </c>
-      <c r="B22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" t="s">
-        <v>123</v>
-      </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F22" s="7">
         <v>0.05</v>
       </c>
       <c r="G22" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="L22" t="s">
         <v>33</v>
@@ -1633,39 +1633,39 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G23" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G24" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="B25" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="I27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1679,7 +1679,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C10" sqref="C10:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1697,7 +1697,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
@@ -1714,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>16</v>
@@ -1972,25 +1972,25 @@
         <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I1" s="1"/>
       <c r="K1" s="1"/>
@@ -2000,13 +2000,13 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>65</v>
@@ -2018,7 +2018,7 @@
         <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2029,7 +2029,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -2058,7 +2058,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>68</v>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2078,13 +2078,13 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>63</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2110,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
@@ -2127,13 +2127,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -2162,7 +2162,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>3</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -2194,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -2261,7 +2261,7 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2269,20 +2269,20 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="C16" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="6:7" ht="185.25">
       <c r="F21" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="6:7">
@@ -2311,36 +2311,36 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2351,45 +2351,45 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -2466,17 +2466,17 @@
     </row>
     <row r="21" spans="1:1" ht="15">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2487,108 +2487,121 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15">
       <c r="A1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
+        <v>179</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
+        <v>180</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
insert tables definition for login and register
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20400" windowHeight="8010" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20400" windowHeight="8010" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="4" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Meal Pack &amp; Weekly planner" sheetId="7" r:id="rId6"/>
     <sheet name="Order to chef" sheetId="5" r:id="rId7"/>
     <sheet name="Pages" sheetId="8" r:id="rId8"/>
+    <sheet name="CRUD Operations Guide" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="227">
   <si>
     <t>RoleName</t>
   </si>
@@ -633,6 +634,75 @@
   </si>
   <si>
     <t>(Dashboard)Take my own order or Cancel order</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>create(Add user)</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Get(Profiles)</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Chef Registration</t>
+  </si>
+  <si>
+    <t>Read or Fetch</t>
+  </si>
+  <si>
+    <t>Get Profile</t>
+  </si>
+  <si>
+    <t>Update Profile</t>
+  </si>
+  <si>
+    <t>Post/Put</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>LoginDetails</t>
+  </si>
+  <si>
+    <t>API Response</t>
+  </si>
+  <si>
+    <t>200, message</t>
+  </si>
+  <si>
+    <t>User basic and address details</t>
+  </si>
+  <si>
+    <t>Chef basic and address details</t>
+  </si>
+  <si>
+    <t>Get( Chef Profiles)</t>
   </si>
 </sst>
 </file>
@@ -710,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -726,6 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,7 +1071,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1739,9 +1810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -2676,7 +2745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2790,4 +2859,251 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="E6" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="E9" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="E12" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="E13" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="E16" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="E17" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="E20" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="E21" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="E25" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="E26" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>